<commit_message>
Update gravity, just need projection of force
</commit_message>
<xml_diff>
--- a/Branch grav/Masses astres.xlsx
+++ b/Branch grav/Masses astres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mael2\Desktop\Git\Python\Branch grav\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A968B6-182E-4E8B-A1EC-3E9E9A33A25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7C86D4-959A-4434-B63B-C213BF49397B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1846,8 +1846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2951,7 +2951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD632101-F391-4EA6-87B1-6F8AAB6666B5}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="101" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="101" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Gravity + 2 planets
</commit_message>
<xml_diff>
--- a/Branch grav/Masses astres.xlsx
+++ b/Branch grav/Masses astres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mael2\Desktop\Git\Python\Branch grav\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6500FEE-396B-4C19-B4E2-8D0E85C01CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEE4726-25BB-42AD-AF23-FB957FF98891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="70">
   <si>
     <t>Astres</t>
   </si>
@@ -96,9 +96,6 @@
     <t>7.23</t>
   </si>
   <si>
-    <t>OrbitRadius</t>
-  </si>
-  <si>
     <t>scale</t>
   </si>
   <si>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>Période de rotation (h)</t>
+  </si>
+  <si>
+    <t>Jour</t>
   </si>
 </sst>
 </file>
@@ -330,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,12 +357,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDEBF7"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -457,15 +475,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -531,13 +540,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -587,9 +633,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -597,9 +640,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -611,19 +651,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -642,9 +682,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -655,9 +692,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -670,31 +704,70 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -703,19 +776,29 @@
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="48">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color auto="1"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -729,24 +812,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
@@ -764,6 +830,12 @@
         <color auto="1"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
@@ -788,7 +860,53 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
@@ -812,9 +930,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -827,8 +951,15 @@
       <font>
         <color auto="1"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -837,16 +968,52 @@
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
       <font>
         <color auto="1"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -855,8 +1022,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -872,13 +1037,25 @@
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
     </dxf>
     <dxf>
       <font>
         <color auto="1"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -887,82 +1064,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -977,7 +1078,76 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -1504,78 +1674,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}" name="Tableau2" displayName="Tableau2" ref="A1:L21" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}" name="Tableau2" displayName="Tableau2" ref="A1:L21" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44">
   <autoFilter ref="A1:L21" xr:uid="{524A4480-6DAB-4CB9-8F9A-6D7582E76A58}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A3C56C48-4D56-4E78-8EAC-8A8834CCB7B6}" name="Astres" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{0ACD23B6-9D0A-41BC-9D2A-22A123127B9A}" name="Masse" dataDxfId="41">
+    <tableColumn id="1" xr3:uid="{A3C56C48-4D56-4E78-8EAC-8A8834CCB7B6}" name="Astres" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{0ACD23B6-9D0A-41BC-9D2A-22A123127B9A}" name="Masse" dataDxfId="42">
       <calculatedColumnFormula>1.988*10^30</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5449565D-8FF5-4D07-BC9E-A81B7DCC7C09}" name="Diamètre (km)" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{2859AEC0-DB80-4F8A-8611-2D1CB99408B1}" name="Aplatissement" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{5449565D-8FF5-4D07-BC9E-A81B7DCC7C09}" name="Diamètre (km)" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{2859AEC0-DB80-4F8A-8611-2D1CB99408B1}" name="Aplatissement" dataDxfId="40">
       <calculatedColumnFormula>9*10^-6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Angle de rotation (deg)" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{F49A900E-B0EE-48B7-858F-35EC2942B732}" name="vitesse rotation équateur (km/jour terrestre)" dataDxfId="37">
+    <tableColumn id="6" xr3:uid="{FEFB98A5-F681-4A28-8656-83E81E4A53E3}" name="Angle de rotation (deg)" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{F49A900E-B0EE-48B7-858F-35EC2942B732}" name="vitesse rotation équateur (km/jour terrestre)" dataDxfId="38">
       <calculatedColumnFormula>24*24*60*60</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur (rad/Jour terrestre)" dataDxfId="36">
+    <tableColumn id="7" xr3:uid="{7B87A2BE-ADED-4EC7-90F4-82312C153D69}" name="vitesse rotation équateur (rad/Jour terrestre)" dataDxfId="37">
       <calculatedColumnFormula>DEGREES((F2*1000/3600)/(C2*1000/2))/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="Distance au soleil" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{8BA55CA0-627D-44EB-B07B-B27C2C506AD3}" name="Distance planète-satellite" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{8E2EBB81-110D-4D53-8EB8-4CFC858D462C}" name="Temps de rotation sur elle-même" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{46007689-E22E-408A-95A0-42C987AB8891}" name="Période de rotation (h)" dataDxfId="32"/>
-    <tableColumn id="12" xr3:uid="{CEB4B556-C34F-49FE-AE7D-1C42DB00465B}" name="Période de révolution (Jour terrestre" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{2C9717ED-55F0-43A9-8BF0-C1A01A73941C}" name="Distance au soleil" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{8BA55CA0-627D-44EB-B07B-B27C2C506AD3}" name="Distance planète-satellite" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{8E2EBB81-110D-4D53-8EB8-4CFC858D462C}" name="Temps de rotation sur elle-même" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{46007689-E22E-408A-95A0-42C987AB8891}" name="Période de rotation (h)" dataDxfId="33"/>
+    <tableColumn id="12" xr3:uid="{CEB4B556-C34F-49FE-AE7D-1C42DB00465B}" name="Période de révolution (Jour terrestre" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A25:G45" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}" name="Tableau24" displayName="Tableau24" ref="A25:G45" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28">
   <autoFilter ref="A25:G45" xr:uid="{6B08AFF7-E6AC-487E-A862-54025ABD7D5C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{57D8D285-6390-4ADD-8C08-C6E8212288A7}" name="Astres" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{9AA0953F-EB7A-4A32-8A2C-59A3B7D54DD6}" name="Masse" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{42C928A3-CDC0-401D-BBEB-DBDE9C296C9E}" name="Diamètre" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{F3774F47-11B7-41CC-BD67-B0851461EE8E}" name="Aplatissement" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{B4AE3617-38DD-4C16-A173-5946879F54C9}" name="Distance soleil" dataDxfId="23">
       <calculatedColumnFormula>H2*$C$23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{126EF6A9-B272-4BB1-AC3A-3BAF656E5D0E}" name="Distance planète satellite" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{C1001996-59B6-404E-967B-839EFC3F25BB}" name="vitesse rotation équateur (km/h)" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{126EF6A9-B272-4BB1-AC3A-3BAF656E5D0E}" name="Distance planète satellite" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}" name="Tableau242" displayName="Tableau242" ref="A1:P21" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
-  <autoFilter ref="A1:P21" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}"/>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{EDE95679-AC5E-459B-B3E8-463BBC0A2BCF}" name="Astres" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{1543D1AE-2916-4C13-B130-4C9C188F65FA}" name="position x" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{BDE35151-E2B7-4D06-8610-409F0E9CE7A8}" name="position y" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{66091E47-CC13-44CA-922F-02228188114E}" name="position z" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{A0A9109F-3A5E-4113-B0C4-45A17BDE5075}" name="vitesse x (m/s)" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}" name="Tableau242" displayName="Tableau242" ref="A1:Q21" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17">
+  <autoFilter ref="A1:Q21" xr:uid="{CE3AC303-40F0-41E2-BA80-E1255A59C86D}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{EDE95679-AC5E-459B-B3E8-463BBC0A2BCF}" name="Astres" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{D0B2E9DF-29DF-408C-8213-3AD64854BC13}" name="scale" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{511C8A8E-79AC-4372-A019-C8C95FAF13DF}" name="Texture" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{1543D1AE-2916-4C13-B130-4C9C188F65FA}" name="position x" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{BDE35151-E2B7-4D06-8610-409F0E9CE7A8}" name="position y" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{66091E47-CC13-44CA-922F-02228188114E}" name="position z" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{A0A9109F-3A5E-4113-B0C4-45A17BDE5075}" name="vitesse x (m/s)" dataDxfId="6">
       <calculatedColumnFormula>360/365</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1FB021ED-D2AE-4B20-9894-A1A7B535AF42}" name="vitesse y" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{1FB021ED-D2AE-4B20-9894-A1A7B535AF42}" name="vitesse y" dataDxfId="11"/>
     <tableColumn id="8" xr3:uid="{6447372A-4624-4464-9007-45A417812819}" name="vitesse z" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{BEAF4F8A-6F7B-4128-8128-A05793BBD938}" name="rotation x" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{B028B5E1-AA94-4521-955D-E61AE895B0ED}" name="rotation y" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{43855469-E423-4784-A5C9-DD6167279A62}" name="rotation z" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{8F5F32B2-D8F6-44B9-956D-C5403B260C0B}" name="OrbitRadius" dataDxfId="5">
-      <calculatedColumnFormula>Tableau242[[#This Row],[position x]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{90418A25-9A76-4ED3-861C-BA83D4A59328}" name="rotation speed x" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{D7830255-2F24-444E-9022-19DC045D5D90}" name="rotation speed y " dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{BEAF4F8A-6F7B-4128-8128-A05793BBD938}" name="rotation x" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{B028B5E1-AA94-4521-955D-E61AE895B0ED}" name="rotation y" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{43855469-E423-4784-A5C9-DD6167279A62}" name="rotation z" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{90418A25-9A76-4ED3-861C-BA83D4A59328}" name="rotation speed x" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{D7830255-2F24-444E-9022-19DC045D5D90}" name="rotation speed y " dataDxfId="2">
       <calculatedColumnFormula>-360/24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{A8BA6684-B306-497B-A744-8A1D3880FB82}" name="rotation speed z" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{D0B2E9DF-29DF-408C-8213-3AD64854BC13}" name="scale" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{511C8A8E-79AC-4372-A019-C8C95FAF13DF}" name="Texture" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{A8BA6684-B306-497B-A744-8A1D3880FB82}" name="rotation speed z" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{B03DB22F-765F-4F06-AEAD-65CC10F8BCF0}" name="Masse" dataDxfId="1">
+      <calculatedColumnFormula>5.9736 * 10^24</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="17" xr3:uid="{5DA3F3EA-DE7C-43C4-8D80-21CB3170CB56}" name="Jour" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1846,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="A8:XFD8"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1859,7 +2030,7 @@
     <col min="5" max="5" width="31.88671875" customWidth="1"/>
     <col min="6" max="6" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29" style="44" customWidth="1"/>
+    <col min="8" max="8" width="29" style="40" customWidth="1"/>
     <col min="9" max="9" width="26.109375" customWidth="1"/>
     <col min="10" max="10" width="39.5546875" customWidth="1"/>
     <col min="11" max="11" width="34.88671875" bestFit="1" customWidth="1"/>
@@ -1874,7 +2045,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>5</v>
@@ -1883,25 +2054,25 @@
         <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>62</v>
+      <c r="K1" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1930,11 +2101,11 @@
         <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (h)]])</f>
         <v>0.23271056693257727</v>
       </c>
-      <c r="H2" s="38">
+      <c r="H2" s="35">
         <v>0</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4">
@@ -1968,11 +2139,11 @@
         <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (h)]])</f>
         <v>0.1071301842656366</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="35">
         <v>57000000</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4">
@@ -2008,11 +2179,11 @@
         <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (h)]])</f>
         <v>2.5855665640013112E-2</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="35">
         <v>108000000</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4">
@@ -2049,11 +2220,11 @@
         <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (h)]])</f>
         <v>6.2831853071795862</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="35">
         <v>149597887.5</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4">
@@ -2089,12 +2260,12 @@
         <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (h)]])</f>
         <v>6.1056336639072768</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="35">
         <f>227.944*10^6</f>
         <v>227944000</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4">
@@ -2117,7 +2288,7 @@
         <f>71492*2</f>
         <v>142984</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="30">
         <v>6.4869999999999997E-2</v>
       </c>
       <c r="E7" s="9">
@@ -2131,12 +2302,12 @@
         <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (h)]])</f>
         <v>15.281145934563177</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="35">
         <f>778.34 *10^6</f>
         <v>778340000</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4">
@@ -2155,14 +2326,14 @@
         <f>1.0243 * 10^26</f>
         <v>1.0243000000000001E+26</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="31">
         <f>24764*2</f>
         <v>49528</v>
       </c>
       <c r="D8" s="10">
         <v>9.7960000000000005E-2</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="31">
         <v>27</v>
       </c>
       <c r="F8" s="9">
@@ -2173,11 +2344,11 @@
         <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (h)]])</f>
         <v>0.61401204995402969</v>
       </c>
-      <c r="H8" s="38">
+      <c r="H8" s="35">
         <v>1426700000</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4">
@@ -2200,7 +2371,7 @@
         <f>25559*2</f>
         <v>51118</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="32">
         <v>2.2929999999999999E-2</v>
       </c>
       <c r="E9" s="9">
@@ -2214,11 +2385,11 @@
         <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (h)]])</f>
         <v>8.4012154827953207</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="35">
         <v>2870700000</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4">
@@ -2241,7 +2412,7 @@
         <f>24764*2</f>
         <v>49528</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="32">
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="E10" s="9">
@@ -2255,11 +2426,11 @@
         <f xml:space="preserve">  (2*PI()/Tableau2[[#This Row],[Période de rotation (h)]])</f>
         <v>9.3346838697725776</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="35">
         <v>4498400000</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4">
@@ -2271,18 +2442,18 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
@@ -2305,23 +2476,23 @@
         <v>16.7</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>39</v>
       </c>
       <c r="I12" s="9">
         <v>384400</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
-        <v>29</v>
+      <c r="A13" s="24" t="s">
+        <v>28</v>
       </c>
       <c r="B13" s="9">
         <f>4.8 * 10^22</f>
@@ -2332,7 +2503,7 @@
         <v>3121.6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="9">
         <v>0.46899999999999997</v>
@@ -2342,24 +2513,24 @@
         <v>115.37406620524585</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="38">
+        <v>42</v>
+      </c>
+      <c r="H13" s="35">
         <f>270*10^6</f>
         <v>270000000</v>
       </c>
-      <c r="I13" s="24">
+      <c r="I13" s="22">
         <v>671000</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
-        <v>30</v>
+      <c r="A14" s="23" t="s">
+        <v>29</v>
       </c>
       <c r="B14" s="9">
         <f>8.9319*10^22</f>
@@ -2370,7 +2541,7 @@
         <v>3643.2</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="9">
         <v>3.5999999999999997E-2</v>
@@ -2380,24 +2551,24 @@
         <v>269.30471424843137</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="38">
+        <v>42</v>
+      </c>
+      <c r="H14" s="35">
         <f>778*10^6</f>
         <v>778000000</v>
       </c>
       <c r="I14" s="9">
         <v>442000</v>
       </c>
-      <c r="J14" s="24" t="s">
-        <v>47</v>
+      <c r="J14" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
-        <v>31</v>
+      <c r="A15" s="24" t="s">
+        <v>30</v>
       </c>
       <c r="B15" s="9">
         <f>1.2 * 10^17</f>
@@ -2405,22 +2576,22 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="9"/>
       <c r="G15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="39"/>
+        <v>42</v>
+      </c>
+      <c r="H15" s="36"/>
       <c r="I15" s="5"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
-        <v>32</v>
+      <c r="A16" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="B16" s="9">
         <f>1.4819*10^23</f>
@@ -2428,22 +2599,22 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="9"/>
       <c r="G16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" s="39"/>
+        <v>42</v>
+      </c>
+      <c r="H16" s="36"/>
       <c r="I16" s="5"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
-        <v>33</v>
+      <c r="A17" s="26" t="s">
+        <v>32</v>
       </c>
       <c r="B17" s="9">
         <f>1.88*10^21</f>
@@ -2451,22 +2622,22 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="9"/>
       <c r="G17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="38"/>
+        <v>42</v>
+      </c>
+      <c r="H17" s="35"/>
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
-        <v>34</v>
+      <c r="A18" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="B18" s="9">
         <f>1.096 * 10^21</f>
@@ -2477,7 +2648,7 @@
         <v>1118</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="5">
         <v>2E-3</v>
@@ -2486,23 +2657,23 @@
         <v>56.73</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" s="24">
+        <v>42</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="22">
         <v>377400</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
-        <v>35</v>
+      <c r="A19" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="B19" s="11">
         <f>2.306518 * 10^21</f>
@@ -2510,22 +2681,22 @@
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="9"/>
       <c r="G19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H19" s="38"/>
+        <v>42</v>
+      </c>
+      <c r="H19" s="35"/>
       <c r="I19" s="5"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="27" t="s">
-        <v>36</v>
+      <c r="A20" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="B20" s="9">
         <f>2.14 * 10^22</f>
@@ -2533,22 +2704,22 @@
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="9"/>
       <c r="G20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="38"/>
+        <v>42</v>
+      </c>
+      <c r="H20" s="35"/>
       <c r="I20" s="5"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="29" t="s">
-        <v>37</v>
+      <c r="A21" s="27" t="s">
+        <v>36</v>
       </c>
       <c r="B21" s="9">
         <f>1.29*10^22</f>
@@ -2556,30 +2727,30 @@
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="38"/>
+        <v>42</v>
+      </c>
+      <c r="H21" s="35"/>
       <c r="I21" s="5"/>
       <c r="J21" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="5"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="37"/>
+      <c r="H22" s="34"/>
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2615,8 +2786,8 @@
       <c r="F25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="23" t="s">
-        <v>42</v>
+      <c r="G25" s="21" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2628,12 +2799,12 @@
         <v>100</v>
       </c>
       <c r="D26" s="7"/>
-      <c r="E26" s="50">
+      <c r="E26" s="44">
         <v>0</v>
       </c>
       <c r="F26" s="9"/>
-      <c r="G26" s="31" t="s">
-        <v>43</v>
+      <c r="G26" s="29" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -2646,13 +2817,13 @@
         <v>0.35035944981058154</v>
       </c>
       <c r="D27" s="10"/>
-      <c r="E27" s="47">
+      <c r="E27" s="42">
         <f>H3*$D$23+100</f>
         <v>105.7</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -2665,13 +2836,13 @@
         <v>0.8690844441380815</v>
       </c>
       <c r="D28" s="10"/>
-      <c r="E28" s="47">
+      <c r="E28" s="42">
         <f t="shared" ref="E28:E34" si="2">H4*$D$23+100</f>
         <v>110.8</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -2684,13 +2855,13 @@
         <v>0.91594891590626437</v>
       </c>
       <c r="D29" s="10"/>
-      <c r="E29" s="47">
+      <c r="E29" s="42">
         <f t="shared" si="2"/>
         <v>114.95978875</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -2703,13 +2874,13 @@
         <v>0.48769139302239412</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="47">
+      <c r="E30" s="42">
         <f t="shared" si="2"/>
         <v>122.7944</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -2722,13 +2893,13 @@
         <v>10.266794190211131</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="47">
+      <c r="E31" s="42">
         <f t="shared" si="2"/>
         <v>177.834</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -2741,13 +2912,13 @@
         <v>3.5562984855143016</v>
       </c>
       <c r="D32" s="5"/>
-      <c r="E32" s="47">
+      <c r="E32" s="42">
         <f t="shared" si="2"/>
         <v>242.67</v>
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2760,13 +2931,13 @@
         <v>3.6704665236335017</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="47">
+      <c r="E33" s="42">
         <f t="shared" si="2"/>
         <v>387.07</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2779,23 +2950,23 @@
         <v>3.5562984855143016</v>
       </c>
       <c r="D34" s="5"/>
-      <c r="E34" s="47">
+      <c r="E34" s="42">
         <f t="shared" si="2"/>
         <v>549.83999999999992</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
@@ -2812,8 +2983,8 @@
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="s">
-        <v>29</v>
+      <c r="A37" s="24" t="s">
+        <v>28</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -2823,8 +2994,8 @@
       <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="25" t="s">
-        <v>30</v>
+      <c r="A38" s="23" t="s">
+        <v>29</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -2834,8 +3005,8 @@
       <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="26" t="s">
-        <v>31</v>
+      <c r="A39" s="24" t="s">
+        <v>30</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -2845,8 +3016,8 @@
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="27" t="s">
-        <v>32</v>
+      <c r="A40" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -2856,8 +3027,8 @@
       <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="28" t="s">
-        <v>33</v>
+      <c r="A41" s="26" t="s">
+        <v>32</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="9"/>
@@ -2867,8 +3038,8 @@
       <c r="G41" s="5"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="27" t="s">
-        <v>34</v>
+      <c r="A42" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="11">
@@ -2881,8 +3052,8 @@
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="28" t="s">
-        <v>35</v>
+      <c r="A43" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -2892,8 +3063,8 @@
       <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="27" t="s">
-        <v>36</v>
+      <c r="A44" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -2903,8 +3074,8 @@
       <c r="G44" s="5"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="29" t="s">
-        <v>37</v>
+      <c r="A45" s="27" t="s">
+        <v>36</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -2949,1070 +3120,1071 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD632101-F391-4EA6-87B1-6F8AAB6666B5}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="10" width="19.88671875" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" style="44" customWidth="1"/>
-    <col min="14" max="14" width="20.6640625" customWidth="1"/>
-    <col min="15" max="15" width="26.88671875" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="35" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="M1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>20</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="43">
+        <v>100</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="52">
         <f>Feuil1!E26</f>
         <v>0</v>
       </c>
-      <c r="C2" s="9">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0</v>
-      </c>
-      <c r="E2" s="8">
-        <v>0</v>
-      </c>
-      <c r="F2" s="9">
-        <v>0</v>
-      </c>
-      <c r="G2" s="38">
-        <v>0</v>
-      </c>
-      <c r="H2" s="36">
-        <v>7.23</v>
-      </c>
-      <c r="I2" s="9">
-        <v>0</v>
-      </c>
-      <c r="J2" s="9">
-        <v>0</v>
-      </c>
-      <c r="K2" s="8">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="9">
-        <v>0</v>
-      </c>
-      <c r="M2" s="51">
-        <v>0.23271056700000001</v>
-      </c>
-      <c r="N2" s="9">
-        <v>0</v>
-      </c>
-      <c r="O2" s="49">
-        <v>100</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="53">
+        <v>0</v>
+      </c>
+      <c r="F2" s="53">
+        <v>0</v>
+      </c>
+      <c r="G2" s="50">
+        <v>0</v>
+      </c>
+      <c r="H2" s="51">
+        <v>0</v>
+      </c>
+      <c r="I2" s="51">
+        <v>0</v>
+      </c>
+      <c r="J2" s="59">
+        <v>7.25</v>
+      </c>
+      <c r="K2" s="56">
+        <v>0</v>
+      </c>
+      <c r="L2" s="56">
+        <v>0</v>
+      </c>
+      <c r="M2" s="60">
+        <v>0</v>
+      </c>
+      <c r="N2" s="61">
+        <v>-1</v>
+      </c>
+      <c r="O2" s="60">
+        <v>0</v>
+      </c>
+      <c r="P2" s="35">
+        <v>1.9884E+27</v>
+      </c>
+      <c r="Q2" s="49">
+        <v>2192832</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9">
-        <v>106</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0</v>
-      </c>
-      <c r="G3" s="38">
-        <v>0</v>
-      </c>
-      <c r="H3" s="37">
-        <v>0.03</v>
-      </c>
-      <c r="I3" s="9">
-        <v>0</v>
-      </c>
-      <c r="J3" s="9">
-        <v>0</v>
-      </c>
-      <c r="K3" s="48">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>106</v>
-      </c>
-      <c r="L3" s="9">
-        <v>0</v>
-      </c>
-      <c r="M3" s="52">
-        <v>0.107130184</v>
-      </c>
-      <c r="N3" s="9">
-        <v>0</v>
-      </c>
-      <c r="O3" s="49">
+      <c r="B3" s="43">
         <v>0.35034999999999999</v>
       </c>
-      <c r="P3" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="52">
+        <v>69296993029</v>
+      </c>
+      <c r="E3" s="53">
+        <v>8513511681</v>
+      </c>
+      <c r="F3" s="53">
+        <v>0</v>
+      </c>
+      <c r="G3" s="50">
+        <v>0</v>
+      </c>
+      <c r="H3" s="51">
+        <v>0</v>
+      </c>
+      <c r="I3" s="51">
+        <v>38860</v>
+      </c>
+      <c r="J3" s="55">
+        <v>7.0039999999999996</v>
+      </c>
+      <c r="K3" s="56">
+        <v>0</v>
+      </c>
+      <c r="L3" s="56">
+        <v>0</v>
+      </c>
+      <c r="M3" s="60">
+        <v>0</v>
+      </c>
+      <c r="N3" s="62">
+        <v>-1</v>
+      </c>
+      <c r="O3" s="60">
+        <v>0</v>
+      </c>
+      <c r="P3" s="35">
+        <v>3.3009999999999998E+23</v>
+      </c>
+      <c r="Q3" s="49">
+        <v>5067360</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9">
-        <v>111</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0</v>
-      </c>
-      <c r="G4" s="38">
-        <v>0</v>
-      </c>
-      <c r="H4" s="37">
+      <c r="B4" s="43">
+        <v>0.8609</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="52">
+        <v>0</v>
+      </c>
+      <c r="E4" s="53">
+        <v>0</v>
+      </c>
+      <c r="F4" s="53">
+        <v>0</v>
+      </c>
+      <c r="G4" s="50">
+        <v>0</v>
+      </c>
+      <c r="H4" s="51">
+        <v>0</v>
+      </c>
+      <c r="I4" s="51">
+        <v>0</v>
+      </c>
+      <c r="J4" s="55">
         <v>177.36</v>
       </c>
-      <c r="I4" s="9">
-        <v>0</v>
-      </c>
-      <c r="J4" s="9">
-        <v>0</v>
-      </c>
-      <c r="K4" s="48">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>111</v>
-      </c>
-      <c r="L4" s="9">
-        <v>0</v>
-      </c>
-      <c r="M4" s="53">
-        <v>2.5855665999999999E-2</v>
-      </c>
-      <c r="N4" s="9">
-        <v>0</v>
-      </c>
-      <c r="O4" s="49">
-        <v>0.8609</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K4" s="56">
+        <v>0</v>
+      </c>
+      <c r="L4" s="56">
+        <v>0</v>
+      </c>
+      <c r="M4" s="60">
+        <v>0</v>
+      </c>
+      <c r="N4" s="63">
+        <v>0</v>
+      </c>
+      <c r="O4" s="60">
+        <v>0</v>
+      </c>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="49"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="43">
+        <v>0.91090000000000004</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="52">
         <v>152097701000</v>
       </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="54">
-        <v>0</v>
-      </c>
-      <c r="F5" s="38">
-        <v>0</v>
-      </c>
-      <c r="G5" s="38">
+      <c r="E5" s="53">
+        <v>0</v>
+      </c>
+      <c r="F5" s="53">
+        <v>0</v>
+      </c>
+      <c r="G5" s="50">
+        <v>0</v>
+      </c>
+      <c r="H5" s="51">
+        <v>0</v>
+      </c>
+      <c r="I5" s="51">
         <v>29290</v>
       </c>
-      <c r="H5" s="38">
+      <c r="J5" s="56">
         <v>23.45</v>
       </c>
-      <c r="I5" s="9">
-        <v>0</v>
-      </c>
-      <c r="J5" s="9">
-        <v>0</v>
-      </c>
-      <c r="K5" s="48">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>152097701000</v>
-      </c>
-      <c r="L5" s="9">
-        <v>0</v>
-      </c>
-      <c r="M5" s="52">
-        <v>6.2831853070000001</v>
-      </c>
-      <c r="N5" s="9">
-        <v>0</v>
-      </c>
-      <c r="O5" s="49">
-        <v>0.91090000000000004</v>
-      </c>
-      <c r="P5" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K5" s="56">
+        <v>0</v>
+      </c>
+      <c r="L5" s="56">
+        <v>0</v>
+      </c>
+      <c r="M5" s="60">
+        <v>0</v>
+      </c>
+      <c r="N5" s="62">
+        <v>-1</v>
+      </c>
+      <c r="O5" s="60">
+        <v>0</v>
+      </c>
+      <c r="P5" s="49">
+        <v>5.9735999999999995E+24</v>
+      </c>
+      <c r="Q5" s="49">
+        <v>86164.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="9">
-        <v>123</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0</v>
-      </c>
-      <c r="G6" s="38">
-        <v>0</v>
-      </c>
-      <c r="H6" s="38">
+      <c r="B6" s="43">
+        <v>0.48759999999999998</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="52">
+        <v>0</v>
+      </c>
+      <c r="E6" s="53">
+        <v>0</v>
+      </c>
+      <c r="F6" s="53">
+        <v>0</v>
+      </c>
+      <c r="G6" s="50">
+        <v>0</v>
+      </c>
+      <c r="H6" s="51">
+        <v>0</v>
+      </c>
+      <c r="I6" s="51">
+        <v>0</v>
+      </c>
+      <c r="J6" s="56">
         <v>25</v>
       </c>
-      <c r="I6" s="9">
-        <v>0</v>
-      </c>
-      <c r="J6" s="9">
-        <v>0</v>
-      </c>
-      <c r="K6" s="48">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>123</v>
-      </c>
-      <c r="L6" s="9">
-        <v>0</v>
-      </c>
-      <c r="M6" s="53">
-        <v>6.105633664</v>
-      </c>
-      <c r="N6" s="9">
-        <v>0</v>
-      </c>
-      <c r="O6" s="49">
-        <v>0.48759999999999998</v>
-      </c>
-      <c r="P6" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K6" s="56">
+        <v>0</v>
+      </c>
+      <c r="L6" s="56">
+        <v>0</v>
+      </c>
+      <c r="M6" s="60">
+        <v>0</v>
+      </c>
+      <c r="N6" s="63">
+        <v>0</v>
+      </c>
+      <c r="O6" s="60">
+        <v>0</v>
+      </c>
+      <c r="P6" s="35"/>
+      <c r="Q6" s="49"/>
+      <c r="S6" s="48"/>
+    </row>
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="9">
-        <v>178</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="9">
-        <v>0</v>
-      </c>
-      <c r="G7" s="38">
-        <v>0</v>
-      </c>
-      <c r="H7" s="37">
+      <c r="B7" s="43">
+        <v>10.2667</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="52">
+        <v>0</v>
+      </c>
+      <c r="E7" s="53">
+        <v>0</v>
+      </c>
+      <c r="F7" s="53">
+        <v>0</v>
+      </c>
+      <c r="G7" s="50">
+        <v>0</v>
+      </c>
+      <c r="H7" s="51">
+        <v>0</v>
+      </c>
+      <c r="I7" s="51">
+        <v>0</v>
+      </c>
+      <c r="J7" s="55">
         <v>1.3049999999999999</v>
       </c>
-      <c r="I7" s="9">
-        <v>0</v>
-      </c>
-      <c r="J7" s="9">
-        <v>0</v>
-      </c>
-      <c r="K7" s="48">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>178</v>
-      </c>
-      <c r="L7" s="9">
-        <v>0</v>
-      </c>
-      <c r="M7" s="52">
-        <v>15.281145929999999</v>
-      </c>
-      <c r="N7" s="9">
-        <v>0</v>
-      </c>
-      <c r="O7" s="49">
-        <v>10.2667</v>
-      </c>
-      <c r="P7" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K7" s="56">
+        <v>0</v>
+      </c>
+      <c r="L7" s="56">
+        <v>0</v>
+      </c>
+      <c r="M7" s="60">
+        <v>0</v>
+      </c>
+      <c r="N7" s="62">
+        <v>0</v>
+      </c>
+      <c r="O7" s="60">
+        <v>0</v>
+      </c>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="49"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="10">
-        <v>1506527701000</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0</v>
-      </c>
-      <c r="G8" s="38">
+      <c r="B8" s="43">
+        <v>3.5562</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="52">
+        <v>1505110000000</v>
+      </c>
+      <c r="E8" s="53">
+        <v>65346019204</v>
+      </c>
+      <c r="F8" s="53">
+        <v>0</v>
+      </c>
+      <c r="G8" s="50">
+        <v>0</v>
+      </c>
+      <c r="H8" s="51">
+        <v>0</v>
+      </c>
+      <c r="I8" s="51">
         <v>9140</v>
       </c>
-      <c r="H8" s="37">
-        <v>27</v>
-      </c>
-      <c r="I8" s="9">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9">
-        <v>0</v>
-      </c>
-      <c r="K8" s="48">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>1506527701000</v>
-      </c>
-      <c r="L8" s="9">
-        <v>0</v>
-      </c>
-      <c r="M8" s="53">
-        <v>14.6957644</v>
-      </c>
-      <c r="N8" s="9">
-        <v>0</v>
-      </c>
-      <c r="O8" s="49">
-        <v>3.5562</v>
-      </c>
-      <c r="P8" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J8" s="55">
+        <v>27.73</v>
+      </c>
+      <c r="K8" s="56">
+        <v>0</v>
+      </c>
+      <c r="L8" s="56">
+        <v>0</v>
+      </c>
+      <c r="M8" s="60">
+        <v>0</v>
+      </c>
+      <c r="N8" s="63">
+        <v>-1</v>
+      </c>
+      <c r="O8" s="60">
+        <v>0</v>
+      </c>
+      <c r="P8" s="34">
+        <v>1.0243000000000001E+26</v>
+      </c>
+      <c r="Q8" s="49">
+        <v>36838.800000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="9">
-        <v>387</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="38">
-        <v>0</v>
-      </c>
-      <c r="H9" s="37">
+      <c r="B9" s="43">
+        <v>3.6703999999999999</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="52">
+        <v>0</v>
+      </c>
+      <c r="E9" s="53">
+        <v>0</v>
+      </c>
+      <c r="F9" s="53">
+        <v>0</v>
+      </c>
+      <c r="G9" s="50">
+        <v>0</v>
+      </c>
+      <c r="H9" s="51">
+        <v>0</v>
+      </c>
+      <c r="I9" s="51">
+        <v>0</v>
+      </c>
+      <c r="J9" s="55">
         <v>98.32</v>
       </c>
-      <c r="I9" s="9">
-        <v>0</v>
-      </c>
-      <c r="J9" s="9">
-        <v>0</v>
-      </c>
-      <c r="K9" s="48">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>387</v>
-      </c>
-      <c r="L9" s="52">
-        <v>8.4012154829999997</v>
-      </c>
-      <c r="M9" s="38">
-        <v>0</v>
-      </c>
-      <c r="N9" s="9">
-        <v>0</v>
-      </c>
-      <c r="O9" s="49">
-        <v>3.6703999999999999</v>
-      </c>
-      <c r="P9" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K9" s="56">
+        <v>0</v>
+      </c>
+      <c r="L9" s="56">
+        <v>0</v>
+      </c>
+      <c r="M9" s="62">
+        <v>0</v>
+      </c>
+      <c r="N9" s="60">
+        <v>0</v>
+      </c>
+      <c r="O9" s="60">
+        <v>0</v>
+      </c>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="49"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="9">
-        <v>550</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0</v>
-      </c>
-      <c r="G10" s="38">
-        <v>0</v>
-      </c>
-      <c r="H10" s="39">
+      <c r="B10" s="43">
+        <v>3.5562</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="52">
+        <v>0</v>
+      </c>
+      <c r="E10" s="53">
+        <v>0</v>
+      </c>
+      <c r="F10" s="53">
+        <v>0</v>
+      </c>
+      <c r="G10" s="50">
+        <v>0</v>
+      </c>
+      <c r="H10" s="51">
+        <v>0</v>
+      </c>
+      <c r="I10" s="51">
+        <v>0</v>
+      </c>
+      <c r="J10" s="57">
         <v>28.32</v>
       </c>
-      <c r="I10" s="9">
-        <v>0</v>
-      </c>
-      <c r="J10" s="9">
-        <v>0</v>
-      </c>
-      <c r="K10" s="48">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>550</v>
-      </c>
-      <c r="L10" s="9">
-        <v>0</v>
-      </c>
-      <c r="M10" s="53">
-        <v>9.3346838699999992</v>
-      </c>
-      <c r="N10" s="9">
-        <v>0</v>
-      </c>
-      <c r="O10" s="49">
-        <v>3.5562</v>
-      </c>
-      <c r="P10" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
+      <c r="K10" s="56">
+        <v>0</v>
+      </c>
+      <c r="L10" s="56">
+        <v>0</v>
+      </c>
+      <c r="M10" s="60">
+        <v>0</v>
+      </c>
+      <c r="N10" s="63">
+        <v>0</v>
+      </c>
+      <c r="O10" s="60">
+        <v>0</v>
+      </c>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="49"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="20">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="19">
-        <v>0</v>
-      </c>
-      <c r="M11" s="42"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="21"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="50">
+        <v>0</v>
+      </c>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="60">
+        <v>0</v>
+      </c>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="49"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="52">
         <v>80</v>
       </c>
-      <c r="C12" s="9">
+      <c r="E12" s="53">
         <v>1</v>
       </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-      <c r="H12" s="39">
+      <c r="F12" s="53">
+        <v>0</v>
+      </c>
+      <c r="G12" s="50">
+        <v>0</v>
+      </c>
+      <c r="H12" s="51">
+        <v>0</v>
+      </c>
+      <c r="I12" s="51">
+        <v>0</v>
+      </c>
+      <c r="J12" s="57">
         <v>5.14</v>
       </c>
-      <c r="I12" s="9">
-        <v>0</v>
-      </c>
-      <c r="J12" s="9">
-        <v>0</v>
-      </c>
-      <c r="K12" s="4">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>80</v>
-      </c>
-      <c r="L12" s="9">
-        <v>0</v>
-      </c>
-      <c r="M12" s="38">
+      <c r="K12" s="56">
+        <v>0</v>
+      </c>
+      <c r="L12" s="56">
+        <v>0</v>
+      </c>
+      <c r="M12" s="60">
+        <v>0</v>
+      </c>
+      <c r="N12" s="60">
         <v>16.7</v>
       </c>
-      <c r="N12" s="9">
-        <v>0</v>
-      </c>
-      <c r="O12" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="P12" s="17" t="s">
+      <c r="O12" s="60">
+        <v>0</v>
+      </c>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="49"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0</v>
+      </c>
+      <c r="C13" s="41">
+        <v>0</v>
+      </c>
+      <c r="D13" s="52">
+        <v>0</v>
+      </c>
+      <c r="E13" s="53">
+        <v>0</v>
+      </c>
+      <c r="F13" s="53">
+        <v>0</v>
+      </c>
+      <c r="G13" s="50">
+        <v>0</v>
+      </c>
+      <c r="H13" s="51">
+        <v>0</v>
+      </c>
+      <c r="I13" s="51">
+        <v>0</v>
+      </c>
+      <c r="J13" s="56">
+        <v>0</v>
+      </c>
+      <c r="K13" s="56">
+        <v>0</v>
+      </c>
+      <c r="L13" s="56">
+        <v>0</v>
+      </c>
+      <c r="M13" s="60">
+        <v>0</v>
+      </c>
+      <c r="N13" s="60">
+        <v>0</v>
+      </c>
+      <c r="O13" s="60">
+        <v>0</v>
+      </c>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="49"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0</v>
+      </c>
+      <c r="C14" s="41">
+        <v>0</v>
+      </c>
+      <c r="D14" s="52">
+        <v>0</v>
+      </c>
+      <c r="E14" s="53">
+        <v>0</v>
+      </c>
+      <c r="F14" s="53">
+        <v>0</v>
+      </c>
+      <c r="G14" s="50">
+        <v>0</v>
+      </c>
+      <c r="H14" s="51">
+        <v>0</v>
+      </c>
+      <c r="I14" s="51">
+        <v>0</v>
+      </c>
+      <c r="J14" s="56">
+        <v>0</v>
+      </c>
+      <c r="K14" s="56">
+        <v>0</v>
+      </c>
+      <c r="L14" s="56">
+        <v>0</v>
+      </c>
+      <c r="M14" s="60">
+        <v>0</v>
+      </c>
+      <c r="N14" s="60">
+        <v>0</v>
+      </c>
+      <c r="O14" s="60">
+        <v>0</v>
+      </c>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="49"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0</v>
+      </c>
+      <c r="C15" s="41">
+        <v>0</v>
+      </c>
+      <c r="D15" s="54">
+        <v>0</v>
+      </c>
+      <c r="E15" s="53">
+        <v>0</v>
+      </c>
+      <c r="F15" s="53">
+        <v>0</v>
+      </c>
+      <c r="G15" s="50">
+        <v>0</v>
+      </c>
+      <c r="H15" s="51">
+        <v>0</v>
+      </c>
+      <c r="I15" s="51">
+        <v>0</v>
+      </c>
+      <c r="J15" s="56">
+        <v>0</v>
+      </c>
+      <c r="K15" s="56">
+        <v>0</v>
+      </c>
+      <c r="L15" s="56">
+        <v>0</v>
+      </c>
+      <c r="M15" s="60">
+        <v>0</v>
+      </c>
+      <c r="N15" s="60">
+        <v>0</v>
+      </c>
+      <c r="O15" s="60">
+        <v>0</v>
+      </c>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="49"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0</v>
+      </c>
+      <c r="C16" s="41">
+        <v>0</v>
+      </c>
+      <c r="D16" s="54">
+        <v>0</v>
+      </c>
+      <c r="E16" s="53">
+        <v>0</v>
+      </c>
+      <c r="F16" s="53">
+        <v>0</v>
+      </c>
+      <c r="G16" s="50">
+        <v>0</v>
+      </c>
+      <c r="H16" s="51">
+        <v>0</v>
+      </c>
+      <c r="I16" s="51">
+        <v>0</v>
+      </c>
+      <c r="J16" s="56">
+        <v>0</v>
+      </c>
+      <c r="K16" s="56">
+        <v>0</v>
+      </c>
+      <c r="L16" s="56">
+        <v>0</v>
+      </c>
+      <c r="M16" s="60">
+        <v>0</v>
+      </c>
+      <c r="N16" s="60">
+        <v>0</v>
+      </c>
+      <c r="O16" s="60">
+        <v>0</v>
+      </c>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="49"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0</v>
+      </c>
+      <c r="C17" s="41">
+        <v>0</v>
+      </c>
+      <c r="D17" s="54">
+        <v>0</v>
+      </c>
+      <c r="E17" s="53">
+        <v>0</v>
+      </c>
+      <c r="F17" s="53">
+        <v>0</v>
+      </c>
+      <c r="G17" s="50">
+        <v>0</v>
+      </c>
+      <c r="H17" s="51">
+        <v>0</v>
+      </c>
+      <c r="I17" s="51">
+        <v>0</v>
+      </c>
+      <c r="J17" s="56">
+        <v>0</v>
+      </c>
+      <c r="K17" s="56">
+        <v>0</v>
+      </c>
+      <c r="L17" s="56">
+        <v>0</v>
+      </c>
+      <c r="M17" s="60">
+        <v>0</v>
+      </c>
+      <c r="N17" s="60">
+        <v>0</v>
+      </c>
+      <c r="O17" s="60">
+        <v>0</v>
+      </c>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="49"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="C18" s="46" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="9">
-        <v>0</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
-        <v>0</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0</v>
-      </c>
-      <c r="G13" s="9">
-        <v>0</v>
-      </c>
-      <c r="H13" s="9">
-        <v>0</v>
-      </c>
-      <c r="I13" s="9">
-        <v>0</v>
-      </c>
-      <c r="J13" s="9">
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="9">
-        <v>0</v>
-      </c>
-      <c r="M13" s="9">
-        <v>0</v>
-      </c>
-      <c r="N13" s="9">
-        <v>0</v>
-      </c>
-      <c r="O13" s="9">
-        <v>0</v>
-      </c>
-      <c r="P13" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="9">
-        <v>0</v>
-      </c>
-      <c r="C14" s="9">
-        <v>0</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0</v>
-      </c>
-      <c r="F14" s="9">
-        <v>0</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0</v>
-      </c>
-      <c r="H14" s="9">
-        <v>0</v>
-      </c>
-      <c r="I14" s="9">
-        <v>0</v>
-      </c>
-      <c r="J14" s="9">
-        <v>0</v>
-      </c>
-      <c r="K14" s="9">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="9">
-        <v>0</v>
-      </c>
-      <c r="M14" s="9">
-        <v>0</v>
-      </c>
-      <c r="N14" s="9">
-        <v>0</v>
-      </c>
-      <c r="O14" s="9">
-        <v>0</v>
-      </c>
-      <c r="P14" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9">
-        <v>0</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0</v>
-      </c>
-      <c r="G15" s="9">
-        <v>0</v>
-      </c>
-      <c r="H15" s="9">
-        <v>0</v>
-      </c>
-      <c r="I15" s="9">
-        <v>0</v>
-      </c>
-      <c r="J15" s="9">
-        <v>0</v>
-      </c>
-      <c r="K15" s="9">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="9">
-        <v>0</v>
-      </c>
-      <c r="M15" s="9">
-        <v>0</v>
-      </c>
-      <c r="N15" s="9">
-        <v>0</v>
-      </c>
-      <c r="O15" s="9">
-        <v>0</v>
-      </c>
-      <c r="P15" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0</v>
-      </c>
-      <c r="C16" s="9">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8">
-        <v>0</v>
-      </c>
-      <c r="F16" s="9">
-        <v>0</v>
-      </c>
-      <c r="G16" s="9">
-        <v>0</v>
-      </c>
-      <c r="H16" s="9">
-        <v>0</v>
-      </c>
-      <c r="I16" s="9">
-        <v>0</v>
-      </c>
-      <c r="J16" s="9">
-        <v>0</v>
-      </c>
-      <c r="K16" s="9">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
-      </c>
-      <c r="L16" s="9">
-        <v>0</v>
-      </c>
-      <c r="M16" s="9">
-        <v>0</v>
-      </c>
-      <c r="N16" s="9">
-        <v>0</v>
-      </c>
-      <c r="O16" s="9">
-        <v>0</v>
-      </c>
-      <c r="P16" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="4">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9">
-        <v>0</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8">
-        <v>0</v>
-      </c>
-      <c r="F17" s="9">
-        <v>0</v>
-      </c>
-      <c r="G17" s="9">
-        <v>0</v>
-      </c>
-      <c r="H17" s="9">
-        <v>0</v>
-      </c>
-      <c r="I17" s="9">
-        <v>0</v>
-      </c>
-      <c r="J17" s="9">
-        <v>0</v>
-      </c>
-      <c r="K17" s="9">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="9">
-        <v>0</v>
-      </c>
-      <c r="M17" s="9">
-        <v>0</v>
-      </c>
-      <c r="N17" s="9">
-        <v>0</v>
-      </c>
-      <c r="O17" s="9">
-        <v>0</v>
-      </c>
-      <c r="P17" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="D18" s="54">
+        <v>110</v>
+      </c>
+      <c r="E18" s="53">
+        <v>5</v>
+      </c>
+      <c r="F18" s="53">
+        <v>0</v>
+      </c>
+      <c r="G18" s="50">
+        <v>0</v>
+      </c>
+      <c r="H18" s="51">
+        <v>0</v>
+      </c>
+      <c r="I18" s="51">
+        <v>0</v>
+      </c>
+      <c r="J18" s="58">
+        <v>2E-3</v>
+      </c>
+      <c r="K18" s="56">
+        <v>0</v>
+      </c>
+      <c r="L18" s="56">
+        <v>0</v>
+      </c>
+      <c r="M18" s="60">
+        <v>0</v>
+      </c>
+      <c r="N18" s="60">
+        <v>53.73</v>
+      </c>
+      <c r="O18" s="60">
+        <v>0</v>
+      </c>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="49"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="4">
-        <v>110</v>
-      </c>
-      <c r="C18" s="9">
-        <v>5</v>
-      </c>
-      <c r="D18" s="9">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8">
-        <v>0</v>
-      </c>
-      <c r="F18" s="9">
-        <v>0</v>
-      </c>
-      <c r="G18" s="9">
-        <v>0</v>
-      </c>
-      <c r="H18" s="41">
-        <v>2E-3</v>
-      </c>
-      <c r="I18" s="9">
-        <v>0</v>
-      </c>
-      <c r="J18" s="9">
-        <v>0</v>
-      </c>
-      <c r="K18" s="9">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>110</v>
-      </c>
-      <c r="L18" s="9">
-        <v>0</v>
-      </c>
-      <c r="M18" s="38">
-        <v>53.73</v>
-      </c>
-      <c r="N18" s="9">
-        <v>0</v>
-      </c>
-      <c r="O18" s="9">
-        <v>0.9</v>
-      </c>
-      <c r="P18" s="46" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="B19" s="9">
+        <v>0</v>
+      </c>
+      <c r="C19" s="41">
+        <v>0</v>
+      </c>
+      <c r="D19" s="54">
+        <v>0</v>
+      </c>
+      <c r="E19" s="53">
+        <v>0</v>
+      </c>
+      <c r="F19" s="53">
+        <v>0</v>
+      </c>
+      <c r="G19" s="50">
+        <v>0</v>
+      </c>
+      <c r="H19" s="51">
+        <v>0</v>
+      </c>
+      <c r="I19" s="51">
+        <v>0</v>
+      </c>
+      <c r="J19" s="56">
+        <v>0</v>
+      </c>
+      <c r="K19" s="56">
+        <v>0</v>
+      </c>
+      <c r="L19" s="56">
+        <v>0</v>
+      </c>
+      <c r="M19" s="60">
+        <v>0</v>
+      </c>
+      <c r="N19" s="60">
+        <v>0</v>
+      </c>
+      <c r="O19" s="60">
+        <v>0</v>
+      </c>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="49"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="4">
-        <v>0</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0</v>
-      </c>
-      <c r="D19" s="9">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19" s="9">
-        <v>0</v>
-      </c>
-      <c r="G19" s="9">
-        <v>0</v>
-      </c>
-      <c r="H19" s="9">
-        <v>0</v>
-      </c>
-      <c r="I19" s="9">
-        <v>0</v>
-      </c>
-      <c r="J19" s="9">
-        <v>0</v>
-      </c>
-      <c r="K19" s="9">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
-      </c>
-      <c r="L19" s="9">
-        <v>0</v>
-      </c>
-      <c r="M19" s="9">
-        <v>0</v>
-      </c>
-      <c r="N19" s="9">
-        <v>0</v>
-      </c>
-      <c r="O19" s="9">
-        <v>0</v>
-      </c>
-      <c r="P19" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="9">
+        <v>0</v>
+      </c>
+      <c r="C20" s="41">
+        <v>0</v>
+      </c>
+      <c r="D20" s="54">
+        <v>0</v>
+      </c>
+      <c r="E20" s="53">
+        <v>0</v>
+      </c>
+      <c r="F20" s="53">
+        <v>0</v>
+      </c>
+      <c r="G20" s="50">
+        <v>0</v>
+      </c>
+      <c r="H20" s="51">
+        <v>0</v>
+      </c>
+      <c r="I20" s="51">
+        <v>0</v>
+      </c>
+      <c r="J20" s="56">
+        <v>0</v>
+      </c>
+      <c r="K20" s="56">
+        <v>0</v>
+      </c>
+      <c r="L20" s="56">
+        <v>0</v>
+      </c>
+      <c r="M20" s="60">
+        <v>0</v>
+      </c>
+      <c r="N20" s="60">
+        <v>0</v>
+      </c>
+      <c r="O20" s="60">
+        <v>0</v>
+      </c>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="49"/>
+    </row>
+    <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="4">
-        <v>0</v>
-      </c>
-      <c r="C20" s="9">
-        <v>0</v>
-      </c>
-      <c r="D20" s="9">
-        <v>0</v>
-      </c>
-      <c r="E20" s="8">
-        <v>0</v>
-      </c>
-      <c r="F20" s="9">
-        <v>0</v>
-      </c>
-      <c r="G20" s="9">
-        <v>0</v>
-      </c>
-      <c r="H20" s="9">
-        <v>0</v>
-      </c>
-      <c r="I20" s="9">
-        <v>0</v>
-      </c>
-      <c r="J20" s="9">
-        <v>0</v>
-      </c>
-      <c r="K20" s="9">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
-      </c>
-      <c r="L20" s="9">
-        <v>0</v>
-      </c>
-      <c r="M20" s="9">
-        <v>0</v>
-      </c>
-      <c r="N20" s="9">
-        <v>0</v>
-      </c>
-      <c r="O20" s="9">
-        <v>0</v>
-      </c>
-      <c r="P20" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="4">
-        <v>0</v>
-      </c>
-      <c r="C21" s="9">
-        <v>0</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0</v>
-      </c>
-      <c r="E21" s="8">
-        <v>0</v>
-      </c>
-      <c r="F21" s="9">
-        <v>0</v>
-      </c>
-      <c r="G21" s="9">
-        <v>0</v>
-      </c>
-      <c r="H21" s="9">
-        <v>0</v>
-      </c>
-      <c r="I21" s="9">
-        <v>0</v>
-      </c>
-      <c r="J21" s="9">
-        <v>0</v>
-      </c>
-      <c r="K21" s="9">
-        <f>Tableau242[[#This Row],[position x]]</f>
-        <v>0</v>
-      </c>
-      <c r="L21" s="9">
-        <v>0</v>
-      </c>
-      <c r="M21" s="9">
-        <v>0</v>
-      </c>
-      <c r="N21" s="9">
-        <v>0</v>
-      </c>
-      <c r="O21" s="9">
-        <v>0</v>
-      </c>
-      <c r="P21" s="45">
-        <v>0</v>
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+      <c r="C21" s="47">
+        <v>0</v>
+      </c>
+      <c r="D21" s="54">
+        <v>0</v>
+      </c>
+      <c r="E21" s="53">
+        <v>0</v>
+      </c>
+      <c r="F21" s="53">
+        <v>0</v>
+      </c>
+      <c r="G21" s="50">
+        <v>0</v>
+      </c>
+      <c r="H21" s="51">
+        <v>0</v>
+      </c>
+      <c r="I21" s="51">
+        <v>0</v>
+      </c>
+      <c r="J21" s="56">
+        <v>0</v>
+      </c>
+      <c r="K21" s="56">
+        <v>0</v>
+      </c>
+      <c r="L21" s="56">
+        <v>0</v>
+      </c>
+      <c r="M21" s="60">
+        <v>0</v>
+      </c>
+      <c r="N21" s="60">
+        <v>0</v>
+      </c>
+      <c r="O21" s="60">
+        <v>0</v>
+      </c>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="49"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P23">
+        <f>1988.4*10^24</f>
+        <v>1.9884E+27</v>
+      </c>
+      <c r="Q23">
+        <f>609.12*3600</f>
+        <v>2192832</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <f>69818000000*SIN(RADIANS(7.004))</f>
+        <v>8513511681.3639135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>